<commit_message>
database update 15:04 19.12
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/x64/Debug/cSharpProje.xlsx
+++ b/WindowsFormsApp2/bin/x64/Debug/cSharpProje.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ertu\Desktop\Proje\WindowsFormsApp2\bin\x64\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A1F4D-80AF-40E8-919E-C2F4F748D613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAA87F1-C759-4C1F-85E9-C6E89A3DC31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14027" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="387" yWindow="387" windowWidth="19200" windowHeight="10026" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kaysor" sheetId="1" r:id="rId1"/>
@@ -31220,7 +31220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -31235,7 +31235,7 @@
     <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>508</v>
       </c>
@@ -31255,7 +31255,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>154326</v>
       </c>
@@ -31275,7 +31275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>154327</v>
       </c>
@@ -31295,7 +31295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>154328</v>
       </c>
@@ -31315,7 +31315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>154329</v>
       </c>
@@ -31335,7 +31335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>154330</v>
       </c>
@@ -31355,7 +31355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>154331</v>
       </c>
@@ -31375,7 +31375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>154332</v>
       </c>
@@ -31395,7 +31395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>154333</v>
       </c>
@@ -31415,7 +31415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>154334</v>
       </c>
@@ -31435,7 +31435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>154335</v>
       </c>
@@ -31455,7 +31455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>154336</v>
       </c>
@@ -31475,7 +31475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>154337</v>
       </c>
@@ -31495,7 +31495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>154338</v>
       </c>
@@ -31515,7 +31515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>154339</v>
       </c>
@@ -31535,7 +31535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>154340</v>
       </c>
@@ -31555,7 +31555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>154341</v>
       </c>
@@ -31575,7 +31575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>154342</v>
       </c>
@@ -31595,7 +31595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>154343</v>
       </c>
@@ -31615,7 +31615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.35" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>154344</v>
       </c>
@@ -33865,8 +33865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
14:19 25.12 AKADEMİSYEN ÖĞRENCİ SORGU OKEY (#27)
Co-authored-by: BeratGkhn <beratberkay37baki@gmail.com>
</commit_message>
<xml_diff>
--- a/WindowsFormsApp2/bin/x64/Debug/cSharpProje.xlsx
+++ b/WindowsFormsApp2/bin/x64/Debug/cSharpProje.xlsx
@@ -31652,10 +31652,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" rightToLeft="false">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -31670,7 +31670,7 @@
     <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>498</v>
       </c>
@@ -31690,7 +31690,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="2">
         <v>154326</v>
       </c>
@@ -31710,7 +31710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="2">
         <v>154327</v>
       </c>
@@ -31730,7 +31730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="2">
         <v>154328</v>
       </c>
@@ -31750,7 +31750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="2">
         <v>154329</v>
       </c>
@@ -31770,7 +31770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="A6" s="2">
         <v>154330</v>
       </c>
@@ -31790,7 +31790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="7">
       <c r="A7" s="2">
         <v>154331</v>
       </c>
@@ -31810,7 +31810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="8">
       <c r="A8" s="2">
         <v>154332</v>
       </c>
@@ -31830,7 +31830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="9">
       <c r="A9" s="2">
         <v>154333</v>
       </c>
@@ -31850,7 +31850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="10">
       <c r="A10" s="2">
         <v>154334</v>
       </c>
@@ -31870,7 +31870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="11">
       <c r="A11" s="2">
         <v>154335</v>
       </c>
@@ -31890,7 +31890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="12">
       <c r="A12" s="2">
         <v>154336</v>
       </c>
@@ -31910,7 +31910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="13">
       <c r="A13" s="2">
         <v>154337</v>
       </c>
@@ -31930,7 +31930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="14">
       <c r="A14" s="2">
         <v>154338</v>
       </c>
@@ -31950,7 +31950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="15">
       <c r="A15" s="2">
         <v>154339</v>
       </c>
@@ -31970,7 +31970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="16">
       <c r="A16" s="2">
         <v>154340</v>
       </c>
@@ -31990,7 +31990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="17">
       <c r="A17" s="2">
         <v>154341</v>
       </c>
@@ -32010,7 +32010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="18">
       <c r="A18" s="2">
         <v>154342</v>
       </c>
@@ -32030,7 +32030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="19">
       <c r="A19" s="2">
         <v>154343</v>
       </c>
@@ -32050,7 +32050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="20">
       <c r="A20" s="2">
         <v>154344</v>
       </c>
@@ -32070,7 +32070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="21">
       <c r="A21" s="2">
         <v>154345</v>
       </c>
@@ -32090,7 +32090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="22">
       <c r="A22" s="2">
         <v>154346</v>
       </c>
@@ -32110,7 +32110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="23">
       <c r="A23" s="2">
         <v>154347</v>
       </c>
@@ -32130,7 +32130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="24">
       <c r="A24" s="2">
         <v>154348</v>
       </c>
@@ -32150,7 +32150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="25">
       <c r="A25" s="2">
         <v>154349</v>
       </c>
@@ -32170,7 +32170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="26">
       <c r="A26" s="2">
         <v>154350</v>
       </c>
@@ -32190,7 +32190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="27">
       <c r="A27" s="2">
         <v>154351</v>
       </c>
@@ -32210,7 +32210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="28">
       <c r="A28" s="2">
         <v>154352</v>
       </c>
@@ -32230,7 +32230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="29">
       <c r="A29" s="2">
         <v>154353</v>
       </c>
@@ -32250,7 +32250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="30">
       <c r="A30" s="2">
         <v>154354</v>
       </c>
@@ -32270,7 +32270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="31">
       <c r="A31" s="2">
         <v>154355</v>
       </c>
@@ -32290,7 +32290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="32">
       <c r="A32" s="2">
         <v>154356</v>
       </c>
@@ -32310,7 +32310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="33">
       <c r="A33" s="2">
         <v>154357</v>
       </c>
@@ -32330,7 +32330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="34">
       <c r="A34" s="2">
         <v>154358</v>
       </c>
@@ -32350,7 +32350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="35">
       <c r="A35" s="2">
         <v>154359</v>
       </c>
@@ -32370,7 +32370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="36">
       <c r="A36" s="2">
         <v>154360</v>
       </c>
@@ -32390,7 +32390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="37">
       <c r="A37" s="2">
         <v>154361</v>
       </c>
@@ -32410,7 +32410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="38">
       <c r="A38" s="2">
         <v>154362</v>
       </c>
@@ -32430,7 +32430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="39">
       <c r="A39" s="2">
         <v>154363</v>
       </c>
@@ -32450,7 +32450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="40">
       <c r="A40" s="2">
         <v>154364</v>
       </c>
@@ -32470,7 +32470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="41">
       <c r="A41" s="2">
         <v>154365</v>
       </c>
@@ -32490,7 +32490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="42">
       <c r="A42" s="2">
         <v>154366</v>
       </c>
@@ -32510,7 +32510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="43">
       <c r="A43" s="2">
         <v>154367</v>
       </c>
@@ -32530,7 +32530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="44">
       <c r="A44" s="2">
         <v>154368</v>
       </c>
@@ -32550,7 +32550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="45">
       <c r="A45" s="2">
         <v>154369</v>
       </c>
@@ -32570,7 +32570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="46">
       <c r="A46" s="2">
         <v>154370</v>
       </c>
@@ -32590,7 +32590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="47">
       <c r="A47" s="2">
         <v>154371</v>
       </c>
@@ -32610,7 +32610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="48">
       <c r="A48" s="2">
         <v>154372</v>
       </c>
@@ -32630,7 +32630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="49">
       <c r="A49" s="2">
         <v>154373</v>
       </c>
@@ -32650,7 +32650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="50">
       <c r="A50" s="2">
         <v>154374</v>
       </c>
@@ -32670,7 +32670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="51">
       <c r="A51" s="2">
         <v>154375</v>
       </c>
@@ -32690,7 +32690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="52">
       <c r="A52" s="2">
         <v>154376</v>
       </c>
@@ -32710,7 +32710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="53">
       <c r="A53" s="2">
         <v>154377</v>
       </c>
@@ -32730,7 +32730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="54">
       <c r="A54" s="2">
         <v>154378</v>
       </c>
@@ -32750,7 +32750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="55">
       <c r="A55" s="2">
         <v>154379</v>
       </c>
@@ -32770,7 +32770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="56">
       <c r="A56" s="2">
         <v>154380</v>
       </c>
@@ -32790,7 +32790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="57">
       <c r="A57" s="2">
         <v>154381</v>
       </c>
@@ -32810,7 +32810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="58">
       <c r="A58" s="2">
         <v>154382</v>
       </c>
@@ -32830,7 +32830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="59">
       <c r="A59" s="2">
         <v>154383</v>
       </c>
@@ -32850,7 +32850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="60">
       <c r="A60" s="2">
         <v>154384</v>
       </c>
@@ -32870,7 +32870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="61">
       <c r="A61" s="2">
         <v>154385</v>
       </c>
@@ -32890,7 +32890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="62">
       <c r="A62" s="2">
         <v>154386</v>
       </c>
@@ -32910,7 +32910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="63">
       <c r="A63" s="2">
         <v>154387</v>
       </c>
@@ -32930,7 +32930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="64">
       <c r="A64" s="2">
         <v>154388</v>
       </c>
@@ -32950,7 +32950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="65">
       <c r="A65" s="2">
         <v>154389</v>
       </c>
@@ -32970,7 +32970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="66">
       <c r="A66" s="2">
         <v>154390</v>
       </c>
@@ -32990,7 +32990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="67">
       <c r="A67" s="2">
         <v>154391</v>
       </c>
@@ -33010,7 +33010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="68">
       <c r="A68" s="2">
         <v>154392</v>
       </c>
@@ -33030,7 +33030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="69">
       <c r="A69" s="2">
         <v>154393</v>
       </c>
@@ -33050,7 +33050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="70">
       <c r="A70" s="2">
         <v>154394</v>
       </c>
@@ -33070,7 +33070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="71">
       <c r="A71" s="2">
         <v>154395</v>
       </c>
@@ -33090,7 +33090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="72">
       <c r="A72" s="2">
         <v>154396</v>
       </c>
@@ -33110,7 +33110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="73">
       <c r="A73" s="2">
         <v>154397</v>
       </c>
@@ -33130,7 +33130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="74">
       <c r="A74" s="2">
         <v>154398</v>
       </c>
@@ -33150,7 +33150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="75">
       <c r="A75" s="2">
         <v>154399</v>
       </c>
@@ -33170,7 +33170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="76">
       <c r="A76" s="2">
         <v>154400</v>
       </c>
@@ -33190,7 +33190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="77">
       <c r="A77" s="2">
         <v>154401</v>
       </c>
@@ -33210,7 +33210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="78">
       <c r="A78" s="2">
         <v>154402</v>
       </c>
@@ -33230,7 +33230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="79">
       <c r="A79" s="2">
         <v>154403</v>
       </c>
@@ -33250,7 +33250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="80">
       <c r="A80" s="2">
         <v>154404</v>
       </c>
@@ -33270,7 +33270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="81">
       <c r="A81" s="2">
         <v>154405</v>
       </c>
@@ -33290,7 +33290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="82">
       <c r="A82" s="2">
         <v>154406</v>
       </c>
@@ -33310,7 +33310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="83">
       <c r="A83" s="2">
         <v>154407</v>
       </c>
@@ -33330,7 +33330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="84">
       <c r="A84" s="2">
         <v>154408</v>
       </c>
@@ -33350,7 +33350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="85">
       <c r="A85" s="2">
         <v>154409</v>
       </c>
@@ -33370,7 +33370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="86">
       <c r="A86" s="2">
         <v>154410</v>
       </c>
@@ -33390,7 +33390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="87">
       <c r="A87" s="2">
         <v>154411</v>
       </c>
@@ -33410,7 +33410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="88">
       <c r="A88" s="2">
         <v>154412</v>
       </c>
@@ -33430,7 +33430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="89">
       <c r="A89" s="2">
         <v>154413</v>
       </c>
@@ -33450,7 +33450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="90">
       <c r="A90" s="2">
         <v>154414</v>
       </c>
@@ -33470,7 +33470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="91">
       <c r="A91" s="2">
         <v>154415</v>
       </c>
@@ -33490,7 +33490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="92">
       <c r="A92" s="2">
         <v>154416</v>
       </c>
@@ -33510,7 +33510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="93">
       <c r="A93" s="2">
         <v>154417</v>
       </c>
@@ -33530,7 +33530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="94">
       <c r="A94" s="2">
         <v>154418</v>
       </c>
@@ -33550,7 +33550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="95">
       <c r="A95" s="2">
         <v>154419</v>
       </c>
@@ -33570,7 +33570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="96">
       <c r="A96" s="2">
         <v>154420</v>
       </c>
@@ -33590,7 +33590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="97">
       <c r="A97" s="2">
         <v>154421</v>
       </c>
@@ -33610,7 +33610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="98">
       <c r="A98" s="2">
         <v>154422</v>
       </c>
@@ -33630,7 +33630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="99">
       <c r="A99" s="2">
         <v>154423</v>
       </c>
@@ -33650,7 +33650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="100">
       <c r="A100" s="2">
         <v>154424</v>
       </c>
@@ -33670,7 +33670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="101">
       <c r="A101" s="2">
         <v>154425</v>
       </c>
@@ -33690,7 +33690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="102">
       <c r="A102" s="2">
         <v>154426</v>
       </c>
@@ -33710,7 +33710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="103">
       <c r="A103" s="2">
         <v>154427</v>
       </c>
@@ -33730,7 +33730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="104">
       <c r="A104" s="2">
         <v>154428</v>
       </c>
@@ -33750,7 +33750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="105">
       <c r="A105" s="2">
         <v>154429</v>
       </c>
@@ -33770,7 +33770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="106">
       <c r="A106" s="2">
         <v>154430</v>
       </c>
@@ -33790,7 +33790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="107">
       <c r="A107" s="2">
         <v>154431</v>
       </c>
@@ -33810,7 +33810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="108">
       <c r="A108" s="2">
         <v>154432</v>
       </c>
@@ -33830,7 +33830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="109">
       <c r="A109" s="2">
         <v>154433</v>
       </c>
@@ -33850,7 +33850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="110">
       <c r="A110" s="2">
         <v>154434</v>
       </c>
@@ -33870,7 +33870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="111">
       <c r="A111" s="2">
         <v>154435</v>
       </c>
@@ -33890,7 +33890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="112">
       <c r="A112" s="2">
         <v>154436</v>
       </c>
@@ -33910,7 +33910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="113">
       <c r="A113" s="2">
         <v>154437</v>
       </c>
@@ -33930,7 +33930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="114">
       <c r="A114" s="2">
         <v>154438</v>
       </c>
@@ -33950,7 +33950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="115">
       <c r="A115" s="2">
         <v>154439</v>
       </c>
@@ -33970,7 +33970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="116">
       <c r="A116" s="2">
         <v>154440</v>
       </c>
@@ -33990,7 +33990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="117">
       <c r="A117" s="2">
         <v>154441</v>
       </c>
@@ -34010,7 +34010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="118">
       <c r="A118" s="2">
         <v>154442</v>
       </c>
@@ -34030,7 +34030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="119">
       <c r="A119" s="2">
         <v>154443</v>
       </c>
@@ -34050,7 +34050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="120">
       <c r="A120" s="2">
         <v>154444</v>
       </c>
@@ -34070,7 +34070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="121">
       <c r="A121" s="2">
         <v>154445</v>
       </c>
@@ -34090,7 +34090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="122">
       <c r="A122" s="2">
         <v>154446</v>
       </c>
@@ -34110,7 +34110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="123">
       <c r="A123" s="2">
         <v>154447</v>
       </c>
@@ -34130,7 +34130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="124">
       <c r="A124" s="2">
         <v>154448</v>
       </c>
@@ -34150,7 +34150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="125">
       <c r="A125" s="2">
         <v>154449</v>
       </c>
@@ -34170,7 +34170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="126">
       <c r="A126" s="2">
         <v>154450</v>
       </c>
@@ -34190,7 +34190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="127">
       <c r="A127" s="2">
         <v>154451</v>
       </c>
@@ -34210,7 +34210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="128">
       <c r="A128" s="2">
         <v>154452</v>
       </c>
@@ -34230,7 +34230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="129">
       <c r="A129" s="2">
         <v>154453</v>
       </c>
@@ -34250,7 +34250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="130">
       <c r="A130" s="2">
         <v>154454</v>
       </c>
@@ -34270,7 +34270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="131">
       <c r="A131" s="2">
         <v>154455</v>
       </c>
@@ -34290,7 +34290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="132">
       <c r="A132" s="2">
         <v>154456</v>
       </c>
@@ -34310,7 +34310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="133">
       <c r="A133" s="2">
         <v>154457</v>
       </c>
@@ -34330,7 +34330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="134">
       <c r="A134" s="2">
         <v>154458</v>
       </c>
@@ -34350,7 +34350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="135">
       <c r="A135" s="2">
         <v>154459</v>
       </c>
@@ -34370,7 +34370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="136">
       <c r="A136" s="2">
         <v>154460</v>
       </c>
@@ -34390,7 +34390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="137">
       <c r="A137" s="2">
         <v>154461</v>
       </c>
@@ -34410,7 +34410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="138">
       <c r="A138" s="2">
         <v>154462</v>
       </c>
@@ -34430,7 +34430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25" outlineLevel="0" r="139">
       <c r="A139" s="2">
         <v>154463</v>
       </c>
@@ -34450,7 +34450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row spans="1:6" x14ac:dyDescent="0.25" outlineLevel="0" r="140">
       <c r="A140" s="4">
         <v>123456</v>
       </c>

</xml_diff>